<commit_message>
Tambah Gambar Toko Makanan
</commit_message>
<xml_diff>
--- a/src/data/DataMakanan12Resto.xlsx
+++ b/src/data/DataMakanan12Resto.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITREP\Repo-Kel2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Regawa\Documents\NetBeansProjects\PROYEK1\proyek_kel2\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="7" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Oto Bento" sheetId="1" r:id="rId1"/>
@@ -1469,7 +1469,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1493,6 +1493,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4591,384 +4593,388 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="13"/>
+    <col min="3" max="3" width="9.140625" style="13"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="D1" s="13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="13" t="s">
         <v>391</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="13">
         <v>5000</v>
       </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
       <c r="D2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="13">
         <v>5000</v>
       </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
       <c r="D3">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="13" t="s">
         <v>392</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="13">
         <v>6000</v>
       </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
       <c r="D4">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="13" t="s">
         <v>393</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="13">
         <v>9000</v>
       </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
       <c r="D5">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="13" t="s">
         <v>394</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="13">
         <v>10000</v>
       </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
       <c r="D6">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="13" t="s">
         <v>395</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="13">
         <v>10000</v>
       </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
       <c r="D7">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="13" t="s">
         <v>396</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="13">
         <v>10000</v>
       </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
       <c r="D8">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="13" t="s">
         <v>397</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="13">
         <v>10000</v>
       </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
       <c r="D9">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="13" t="s">
         <v>398</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="13">
         <v>10000</v>
       </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
       <c r="D10">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="13" t="s">
         <v>399</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="13">
         <v>10000</v>
       </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
       <c r="D11">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="13" t="s">
         <v>400</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="13">
         <v>10000</v>
       </c>
-      <c r="C12" t="s">
-        <v>22</v>
-      </c>
       <c r="D12">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="13" t="s">
         <v>401</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="13">
         <v>10000</v>
       </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
       <c r="D13">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="13" t="s">
         <v>402</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="13">
         <v>11000</v>
       </c>
-      <c r="C14" t="s">
-        <v>2</v>
-      </c>
       <c r="D14">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="13" t="s">
         <v>403</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="13">
         <v>14000</v>
       </c>
-      <c r="C15" t="s">
-        <v>2</v>
-      </c>
       <c r="D15">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="13" t="s">
         <v>404</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="13">
         <v>17000</v>
       </c>
-      <c r="C16" t="s">
-        <v>2</v>
-      </c>
       <c r="D16">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="13" t="s">
         <v>405</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="13">
         <v>17000</v>
       </c>
-      <c r="C17" t="s">
-        <v>2</v>
-      </c>
       <c r="D17">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="13" t="s">
         <v>406</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="13">
         <v>18000</v>
       </c>
-      <c r="C18" t="s">
-        <v>2</v>
-      </c>
       <c r="D18">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="13" t="s">
         <v>407</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="13">
         <v>23000</v>
       </c>
-      <c r="C19" t="s">
-        <v>2</v>
-      </c>
       <c r="D19">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="13" t="s">
         <v>408</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="13">
         <v>26000</v>
       </c>
-      <c r="C20" t="s">
-        <v>2</v>
-      </c>
       <c r="D20">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="13" t="s">
         <v>409</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="13">
         <v>28000</v>
       </c>
-      <c r="C21" t="s">
-        <v>2</v>
-      </c>
       <c r="D21">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="13" t="s">
         <v>410</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="13">
         <v>32000</v>
       </c>
-      <c r="C22" t="s">
-        <v>2</v>
-      </c>
       <c r="D22">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="13" t="s">
         <v>411</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="13">
         <v>33000</v>
       </c>
-      <c r="C23" t="s">
-        <v>2</v>
-      </c>
       <c r="D23">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="13">
         <v>33000</v>
       </c>
-      <c r="C24" t="s">
-        <v>2</v>
-      </c>
       <c r="D24">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="13" t="s">
         <v>413</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="13">
         <v>35000</v>
       </c>
-      <c r="C25" t="s">
-        <v>2</v>
-      </c>
       <c r="D25">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="13" t="s">
         <v>414</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="13">
         <v>45000</v>
       </c>
-      <c r="C26" t="s">
-        <v>2</v>
-      </c>
       <c r="D26">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="13" t="s">
         <v>415</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="13">
         <v>55000</v>
-      </c>
-      <c r="C27" t="s">
-        <v>2</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -4983,8 +4989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5686,358 +5692,311 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="9.140625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="13">
         <v>10000</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="B3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="13">
         <v>10000</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="13">
         <v>10000</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B5" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="13">
         <v>19000</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="13">
         <v>20000</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="B7" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="13">
         <v>28000</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="B8" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="13">
         <v>64000</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="B9" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="13">
         <v>69000</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="2">
+      <c r="B10" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="13">
         <v>72000</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="2">
+      <c r="B11" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="13">
         <v>89000</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="2">
+      <c r="B12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="13">
         <v>15000</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="2">
+      <c r="B13" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="13">
         <v>30000</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="2">
+      <c r="B14" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="13">
         <v>35000</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="2">
+      <c r="B15" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="13">
         <v>35000</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="2">
+      <c r="B16" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="13">
         <v>35000</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="2">
+      <c r="B17" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="13">
         <v>35000</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="2">
+      <c r="B18" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="13">
         <v>35000</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="2">
+      <c r="B19" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="13">
         <v>35000</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="2">
+      <c r="B20" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="13">
         <v>35000</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="2">
+      <c r="B21" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="13">
         <v>35000</v>
       </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C26" s="2"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C27" s="2"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C28" s="2"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C29" s="2"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C31" s="2"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C32" s="2"/>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33" s="2"/>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C34" s="2"/>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C35" s="2"/>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C36" s="2"/>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C37" s="2"/>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C38" s="2"/>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C39" s="2"/>
+      <c r="D21" s="13">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:D21">
@@ -6685,7 +6644,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6997,7 +6956,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
@@ -7005,10 +6964,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="3"/>
-    <col min="3" max="3" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="32.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="14"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -7021,599 +6981,555 @@
       <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="5">
+      <c r="B2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="14">
         <v>81000</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="5">
+      <c r="B3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="14">
         <v>43000</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="B4" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="14">
         <v>48000</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="5">
+      <c r="B5" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="14">
         <v>43000</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="5">
+      <c r="B6" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="14">
         <v>42000</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="B7" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="14">
         <v>71000</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="5">
+      <c r="B8" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="14">
         <v>31000</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="5">
+      <c r="B9" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="14">
         <v>40000</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="5">
+      <c r="B10" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="14">
         <v>34000</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="5">
+      <c r="B11" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="14">
         <v>40000</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="5">
+      <c r="B12" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="14">
         <v>16000</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="5">
+      <c r="B13" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="14">
         <v>40000</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="5">
+      <c r="B14" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="14">
         <v>38000</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="5">
+      <c r="B15" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="14">
         <v>32000</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="5">
+      <c r="B16" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="14">
         <v>12000</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="5">
+      <c r="B17" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="14">
         <v>71000</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="5">
+      <c r="B18" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="14">
         <v>81000</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="5">
+      <c r="B19" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="14">
         <v>81000</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="5">
+      <c r="B20" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="14">
         <v>71000</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" s="5">
+      <c r="B21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="14">
         <v>34000</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="5">
+      <c r="B22" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="14">
         <v>34000</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23" s="5">
+      <c r="B23" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="14">
         <v>43000</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" s="5">
+      <c r="B24" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="14">
         <v>81000</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C25" s="5">
+      <c r="B25" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="14">
         <v>26000</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" s="5">
+      <c r="B26" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="14">
         <v>18000</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="5">
+      <c r="B27" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="14">
         <v>40000</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" s="5">
+      <c r="B28" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="14">
         <v>85000</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" s="5">
+      <c r="B29" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="14">
         <v>30000</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30" s="5">
+      <c r="B30" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="14">
         <v>81000</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" s="5">
+      <c r="B31" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="14">
         <v>71000</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C32" s="5">
+      <c r="B32" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="14">
         <v>32000</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C33" s="5">
+      <c r="B33" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="14">
         <v>43000</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D33" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C34" s="5">
+      <c r="B34" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="14">
         <v>6000</v>
       </c>
-      <c r="D34" s="5">
+      <c r="D34" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C35" s="5">
+      <c r="B35" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="14">
         <v>18000</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D35" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C36" s="5">
+      <c r="B36" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="14">
         <v>12000</v>
       </c>
-      <c r="D36" s="5">
+      <c r="D36" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C37" s="5">
+      <c r="B37" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" s="14">
         <v>12000</v>
       </c>
-      <c r="D37" s="5">
+      <c r="D37" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C38" s="5">
+      <c r="B38" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="14">
         <v>12000</v>
       </c>
-      <c r="D38" s="5">
+      <c r="D38" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C39" s="5">
+      <c r="B39" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="14">
         <v>18000</v>
       </c>
-      <c r="D39" s="5">
+      <c r="D39" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C40" s="5">
+      <c r="B40" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" s="14">
         <v>8000</v>
       </c>
-      <c r="D40" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-    </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-    </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-    </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
+      <c r="D40" s="14">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>